<commit_message>
update data to 3/31/2023
</commit_message>
<xml_diff>
--- a/EquityHedging/data/update_data/liq_alts_bmk_data.xlsx
+++ b/EquityHedging/data/update_data/liq_alts_bmk_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nvg9hxp\Documents\Projects\RMP\EquityHedging\data\update_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pforj\Documents\ups\RMP\EquityHedging\data\update_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44FCF81-B743-4BB7-87A5-459E5052A919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD22BA3-7967-4D2D-B938-55584460775F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="2715" windowWidth="28800" windowHeight="15375" xr2:uid="{302BD275-697C-4771-A918-03BF7FE267B6}"/>
+    <workbookView xWindow="4905" yWindow="5145" windowWidth="28110" windowHeight="15660" activeTab="1" xr2:uid="{302BD275-697C-4771-A918-03BF7FE267B6}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -256,6 +256,405 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
+<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <volType type="realTimeData">
+    <main first="bloomberg.rtd">
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C15</stp>
+        <stp>PX_LAST</stp>
+        <tr r="O5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C14</stp>
+        <stp>PX_LAST</stp>
+        <tr r="N5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C17</stp>
+        <stp>PX_LAST</stp>
+        <tr r="Q5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C16</stp>
+        <stp>PX_LAST</stp>
+        <tr r="P5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C11</stp>
+        <stp>PX_LAST</stp>
+        <tr r="K5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C10</stp>
+        <stp>PX_LAST</stp>
+        <tr r="J5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C13</stp>
+        <stp>PX_LAST</stp>
+        <tr r="M5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C12</stp>
+        <stp>PX_LAST</stp>
+        <tr r="L5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C19</stp>
+        <stp>PX_LAST</stp>
+        <tr r="S5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C18</stp>
+        <stp>PX_LAST</stp>
+        <tr r="R5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C25</stp>
+        <stp>PX_LAST</stp>
+        <tr r="Y5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C24</stp>
+        <stp>PX_LAST</stp>
+        <tr r="X5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C26</stp>
+        <stp>PX_LAST</stp>
+        <tr r="Z5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C21</stp>
+        <stp>PX_LAST</stp>
+        <tr r="U5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C20</stp>
+        <stp>PX_LAST</stp>
+        <tr r="T5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C23</stp>
+        <stp>PX_LAST</stp>
+        <tr r="W5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C22</stp>
+        <stp>PX_LAST</stp>
+        <tr r="V5" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|15505813804946371114</stp>
+        <tr r="F7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|17806941702052096784</stp>
+        <tr r="U7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|16282985324127864257</stp>
+        <tr r="R7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|17895663197078668805</stp>
+        <tr r="O7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|10628674081187910092</stp>
+        <tr r="M7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|12755651984071516276</stp>
+        <tr r="I7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|14993532421909430696</stp>
+        <tr r="C7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|14173773038049759993</stp>
+        <tr r="A7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|10282607615152582414</stp>
+        <tr r="Z7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|17889426319144630069</stp>
+        <tr r="Q7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|16467459298265297818</stp>
+        <tr r="L7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|11948652408209093964</stp>
+        <tr r="D7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|18353832827956336096</stp>
+        <tr r="Y7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|4390742966770117848</stp>
+        <tr r="P7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|5397265506728188119</stp>
+        <tr r="H7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|5049773584473586661</stp>
+        <tr r="N7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|5683877689649636667</stp>
+        <tr r="S7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|8858789470707016578</stp>
+        <tr r="J7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|8239745973199805405</stp>
+        <tr r="W7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|2734053279304251766</stp>
+        <tr r="X7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|9278831636327226344</stp>
+        <tr r="G7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|8583426625565047866</stp>
+        <tr r="K7" s="1"/>
+      </tp>
+    </main>
+    <main first="bloomberg.rtd">
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C5</stp>
+        <stp>PX_LAST</stp>
+        <tr r="E5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C4</stp>
+        <stp>PX_LAST</stp>
+        <tr r="D5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C7</stp>
+        <stp>PX_LAST</stp>
+        <tr r="G5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C6</stp>
+        <stp>PX_LAST</stp>
+        <tr r="F5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C3</stp>
+        <stp>PX_LAST</stp>
+        <tr r="C5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C2</stp>
+        <stp>PX_LAST</stp>
+        <tr r="B5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C9</stp>
+        <stp>PX_LAST</stp>
+        <tr r="I5" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>Last Price</v>
+        <stp/>
+        <stp>##V3_BFIELDINFOV12</stp>
+        <stp>[liq_alts_bmk_data.xlsx]data!R5C8</stp>
+        <stp>PX_LAST</stp>
+        <tr r="H5" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|171450380806983985</stp>
+        <tr r="T7" s="1"/>
+      </tp>
+    </main>
+    <main first="bofaddin.rtdserver">
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|741800188608557779</stp>
+        <tr r="V7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|374973041562415077</stp>
+        <tr r="E7" s="1"/>
+      </tp>
+    </main>
+  </volType>
+</volTypes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -555,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96104C0-A0F5-4396-A1EE-ED2FBB5E9388}">
-  <dimension ref="A1:Z188"/>
+  <dimension ref="A1:Z191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA1:AA1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +979,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>44926</v>
+        <v>45016</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -661,105 +1060,105 @@
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B5" t="e">
-        <f ca="1">_xll.BFieldInfo(B$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C5" t="e">
-        <f ca="1">_xll.BFieldInfo(C$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D5" t="e">
-        <f ca="1">_xll.BFieldInfo(D$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E5" t="e">
-        <f ca="1">_xll.BFieldInfo(E$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F5" t="e">
-        <f ca="1">_xll.BFieldInfo(F$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G5" t="e">
-        <f ca="1">_xll.BFieldInfo(G$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="H5" t="e">
-        <f ca="1">_xll.BFieldInfo(H$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I5" t="e">
-        <f ca="1">_xll.BFieldInfo(I$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J5" t="e">
-        <f ca="1">_xll.BFieldInfo(J$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K5" t="e">
-        <f ca="1">_xll.BFieldInfo(K$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="L5" t="e">
-        <f ca="1">_xll.BFieldInfo(L$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M5" t="e">
-        <f ca="1">_xll.BFieldInfo(M$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="N5" t="e">
-        <f ca="1">_xll.BFieldInfo(N$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="O5" t="e">
-        <f ca="1">_xll.BFieldInfo(O$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="P5" t="e">
-        <f ca="1">_xll.BFieldInfo(P$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Q5" t="e">
-        <f ca="1">_xll.BFieldInfo(Q$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="R5" t="e">
-        <f ca="1">_xll.BFieldInfo(R$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="S5" t="e">
-        <f ca="1">_xll.BFieldInfo(S$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="T5" t="e">
-        <f ca="1">_xll.BFieldInfo(T$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="U5" t="e">
-        <f ca="1">_xll.BFieldInfo(U$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="V5" t="e">
-        <f ca="1">_xll.BFieldInfo(V$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="W5" t="e">
-        <f ca="1">_xll.BFieldInfo(W$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="X5" t="e">
-        <f ca="1">_xll.BFieldInfo(X$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Y5" t="e">
-        <f ca="1">_xll.BFieldInfo(Y$6)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Z5" t="e">
-        <f ca="1">_xll.BFieldInfo(Z$6)</f>
-        <v>#NAME?</v>
+      <c r="B5" t="str">
+        <f>_xll.BFieldInfo(B$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="C5" t="str">
+        <f>_xll.BFieldInfo(C$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="D5" t="str">
+        <f>_xll.BFieldInfo(D$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="E5" t="str">
+        <f>_xll.BFieldInfo(E$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="F5" t="str">
+        <f>_xll.BFieldInfo(F$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="G5" t="str">
+        <f>_xll.BFieldInfo(G$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="H5" t="str">
+        <f>_xll.BFieldInfo(H$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="I5" t="str">
+        <f>_xll.BFieldInfo(I$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="J5" t="str">
+        <f>_xll.BFieldInfo(J$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="K5" t="str">
+        <f>_xll.BFieldInfo(K$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="L5" t="str">
+        <f>_xll.BFieldInfo(L$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="M5" t="str">
+        <f>_xll.BFieldInfo(M$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="N5" t="str">
+        <f>_xll.BFieldInfo(N$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="O5" t="str">
+        <f>_xll.BFieldInfo(O$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="P5" t="str">
+        <f>_xll.BFieldInfo(P$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="Q5" t="str">
+        <f>_xll.BFieldInfo(Q$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="R5" t="str">
+        <f>_xll.BFieldInfo(R$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="S5" t="str">
+        <f>_xll.BFieldInfo(S$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="T5" t="str">
+        <f>_xll.BFieldInfo(T$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="U5" t="str">
+        <f>_xll.BFieldInfo(U$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="V5" t="str">
+        <f>_xll.BFieldInfo(V$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="W5" t="str">
+        <f>_xll.BFieldInfo(W$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="X5" t="str">
+        <f>_xll.BFieldInfo(X$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="Y5" t="str">
+        <f>_xll.BFieldInfo(Y$6)</f>
+        <v>Last Price</v>
+      </c>
+      <c r="Z5" t="str">
+        <f>_xll.BFieldInfo(Z$6)</f>
+        <v>Last Price</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -843,108 +1242,108 @@
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="e">
-        <f ca="1">_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=S","cols=2;rows=182")</f>
-        <v>#NAME?</v>
+      <c r="A7" s="1">
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=S","cols=2;rows=185")</f>
+        <v>39416</v>
       </c>
       <c r="B7">
         <v>1270.6300000000001</v>
       </c>
-      <c r="C7" t="e">
-        <f ca="1">_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D7" t="e">
-        <f ca="1">_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E7" t="e">
-        <f ca="1">_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F7" t="e">
-        <f ca="1">_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G7" t="e">
-        <f ca="1">_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="H7" t="e">
-        <f ca="1">_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I7" t="e">
-        <f ca="1">_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J7" t="e">
-        <f ca="1">_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K7" t="e">
-        <f ca="1">_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="L7" t="e">
-        <f ca="1">_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M7" t="e">
-        <f ca="1">_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="N7" t="e">
-        <f ca="1">_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="O7" t="e">
-        <f ca="1">_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="P7" t="e">
-        <f ca="1">_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Q7" t="e">
-        <f ca="1">_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="R7" t="e">
-        <f ca="1">_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="S7" t="e">
-        <f ca="1">_xll.BDH(S$4,S$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="T7" t="e">
-        <f ca="1">_xll.BDH(T$4,T$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="U7" t="e">
-        <f ca="1">_xll.BDH(U$4,U$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="V7" t="e">
-        <f ca="1">_xll.BDH(V$4,V$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="W7" t="e">
-        <f ca="1">_xll.BDH(W$4,W$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="X7" t="e">
-        <f ca="1">_xll.BDH(X$4,X$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Y7" t="e">
-        <f ca="1">_xll.BDH(Y$4,Y$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Z7" t="e">
-        <f ca="1">_xll.BDH(Z$4,Z$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>#NAME?</v>
+      <c r="C7">
+        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>1890.095</v>
+      </c>
+      <c r="D7">
+        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>1175.0999999999999</v>
+      </c>
+      <c r="E7">
+        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>4956.05</v>
+      </c>
+      <c r="F7">
+        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>1242.06</v>
+      </c>
+      <c r="G7">
+        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>169.2372</v>
+      </c>
+      <c r="H7">
+        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>358.60399999999998</v>
+      </c>
+      <c r="I7">
+        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>406.08</v>
+      </c>
+      <c r="J7">
+        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>690.92</v>
+      </c>
+      <c r="K7">
+        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>177.24680000000001</v>
+      </c>
+      <c r="L7">
+        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>7059.31</v>
+      </c>
+      <c r="M7">
+        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>22.87</v>
+      </c>
+      <c r="N7">
+        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>1441.79</v>
+      </c>
+      <c r="O7">
+        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>230.74090000000001</v>
+      </c>
+      <c r="P7">
+        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>86.929199999999994</v>
+      </c>
+      <c r="Q7">
+        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>1740.904</v>
+      </c>
+      <c r="R7">
+        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>1291.96</v>
+      </c>
+      <c r="S7">
+        <f>_xll.BDH(S$4,S$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>1268.96</v>
+      </c>
+      <c r="T7">
+        <f>_xll.BDH(T$4,T$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>1331.55</v>
+      </c>
+      <c r="U7">
+        <f>_xll.BDH(U$4,U$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>1351.68</v>
+      </c>
+      <c r="V7">
+        <f>_xll.BDH(V$4,V$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>1495.05</v>
+      </c>
+      <c r="W7">
+        <f>_xll.BDH(W$4,W$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>1071.01</v>
+      </c>
+      <c r="X7">
+        <f>_xll.BDH(X$4,X$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>1663.27</v>
+      </c>
+      <c r="Y7">
+        <f>_xll.BDH(Y$4,Y$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>1588.29</v>
+      </c>
+      <c r="Z7" t="str">
+        <f>_xll.BDH(Z$4,Z$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=185")</f>
+        <v>#N/A N/A</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -15237,7 +15636,7 @@
         <v>104.1336</v>
       </c>
       <c r="Q186">
-        <v>3103.3780000000002</v>
+        <v>3103.377</v>
       </c>
       <c r="R186">
         <v>1991.28</v>
@@ -15317,7 +15716,7 @@
         <v>104.1336</v>
       </c>
       <c r="Q187">
-        <v>2944.97</v>
+        <v>2945.5120000000002</v>
       </c>
       <c r="R187">
         <v>1892.02</v>
@@ -15355,7 +15754,7 @@
         <v>1266.8900000000001</v>
       </c>
       <c r="C188">
-        <v>3870.047</v>
+        <v>3870.6570000000002</v>
       </c>
       <c r="D188">
         <v>1167.92</v>
@@ -15397,7 +15796,7 @@
         <v>104.1336</v>
       </c>
       <c r="Q188">
-        <v>2939.183</v>
+        <v>2942.846</v>
       </c>
       <c r="R188">
         <v>1891.06</v>
@@ -15421,10 +15820,250 @@
         <v>2027.59</v>
       </c>
       <c r="Y188">
-        <v>2012.87</v>
+        <v>2050.29</v>
       </c>
       <c r="Z188">
-        <v>1736.29</v>
+        <v>1735.79</v>
+      </c>
+    </row>
+    <row r="189" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>44957</v>
+      </c>
+      <c r="B189">
+        <v>1267.28</v>
+      </c>
+      <c r="C189">
+        <v>3817.4569999999999</v>
+      </c>
+      <c r="D189">
+        <v>1168.94</v>
+      </c>
+      <c r="E189">
+        <v>12532.09</v>
+      </c>
+      <c r="F189">
+        <v>1031.5</v>
+      </c>
+      <c r="G189">
+        <v>200.17509999999999</v>
+      </c>
+      <c r="H189">
+        <v>460.55410000000001</v>
+      </c>
+      <c r="I189">
+        <v>792.15</v>
+      </c>
+      <c r="J189">
+        <v>1654.1</v>
+      </c>
+      <c r="K189">
+        <v>111.8001</v>
+      </c>
+      <c r="L189">
+        <v>3492.7080000000001</v>
+      </c>
+      <c r="M189">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="N189">
+        <v>1703.77</v>
+      </c>
+      <c r="O189">
+        <v>280.98469999999998</v>
+      </c>
+      <c r="P189">
+        <v>104.1336</v>
+      </c>
+      <c r="Q189">
+        <v>2919.2489999999998</v>
+      </c>
+      <c r="R189">
+        <v>1872.61</v>
+      </c>
+      <c r="S189">
+        <v>1279.02</v>
+      </c>
+      <c r="T189">
+        <v>1390.72</v>
+      </c>
+      <c r="U189">
+        <v>1469.81</v>
+      </c>
+      <c r="V189">
+        <v>1679.48</v>
+      </c>
+      <c r="W189">
+        <v>907.47</v>
+      </c>
+      <c r="X189">
+        <v>2116.75</v>
+      </c>
+      <c r="Y189">
+        <v>2045.57</v>
+      </c>
+      <c r="Z189">
+        <v>1758.37</v>
+      </c>
+    </row>
+    <row r="190" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>44985</v>
+      </c>
+      <c r="B190">
+        <v>1273.56</v>
+      </c>
+      <c r="C190">
+        <v>3888.33</v>
+      </c>
+      <c r="D190">
+        <v>1166.95</v>
+      </c>
+      <c r="E190">
+        <v>12235.69</v>
+      </c>
+      <c r="F190">
+        <v>964.01</v>
+      </c>
+      <c r="G190">
+        <v>193.0421</v>
+      </c>
+      <c r="H190">
+        <v>445.24340000000001</v>
+      </c>
+      <c r="I190">
+        <v>774.69</v>
+      </c>
+      <c r="J190">
+        <v>1635.33</v>
+      </c>
+      <c r="K190">
+        <v>106.1591</v>
+      </c>
+      <c r="L190">
+        <v>3359.08</v>
+      </c>
+      <c r="M190">
+        <v>20.7</v>
+      </c>
+      <c r="N190">
+        <v>1665.61</v>
+      </c>
+      <c r="O190">
+        <v>286.65769999999998</v>
+      </c>
+      <c r="P190">
+        <v>104.1336</v>
+      </c>
+      <c r="Q190">
+        <v>2981.4229999999998</v>
+      </c>
+      <c r="R190">
+        <v>1907.87</v>
+      </c>
+      <c r="S190">
+        <v>1272.47</v>
+      </c>
+      <c r="T190">
+        <v>1384.21</v>
+      </c>
+      <c r="U190">
+        <v>1460.8</v>
+      </c>
+      <c r="V190">
+        <v>1663.67</v>
+      </c>
+      <c r="W190">
+        <v>896.26</v>
+      </c>
+      <c r="X190">
+        <v>2084.29</v>
+      </c>
+      <c r="Y190">
+        <v>2025.31</v>
+      </c>
+      <c r="Z190">
+        <v>1762.87</v>
+      </c>
+    </row>
+    <row r="191" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>45016</v>
+      </c>
+      <c r="B191">
+        <v>1235.1600000000001</v>
+      </c>
+      <c r="C191">
+        <v>3587.9360000000001</v>
+      </c>
+      <c r="D191">
+        <v>1165.6300000000001</v>
+      </c>
+      <c r="E191">
+        <v>12622.66</v>
+      </c>
+      <c r="F191">
+        <v>990.28</v>
+      </c>
+      <c r="G191">
+        <v>200.1739</v>
+      </c>
+      <c r="H191">
+        <v>459.3227</v>
+      </c>
+      <c r="I191">
+        <v>785.53</v>
+      </c>
+      <c r="J191">
+        <v>1657.25</v>
+      </c>
+      <c r="K191">
+        <v>105.5076</v>
+      </c>
+      <c r="L191">
+        <v>3323.0129999999999</v>
+      </c>
+      <c r="M191">
+        <v>18.7</v>
+      </c>
+      <c r="N191">
+        <v>1691.69</v>
+      </c>
+      <c r="O191">
+        <v>284.00749999999999</v>
+      </c>
+      <c r="P191">
+        <v>104.1336</v>
+      </c>
+      <c r="Q191">
+        <v>2789.4490000000001</v>
+      </c>
+      <c r="R191">
+        <v>1780.84</v>
+      </c>
+      <c r="S191">
+        <v>1264.57</v>
+      </c>
+      <c r="T191">
+        <v>1367.78</v>
+      </c>
+      <c r="U191">
+        <v>1458.79</v>
+      </c>
+      <c r="V191">
+        <v>1637.57</v>
+      </c>
+      <c r="W191">
+        <v>898.67</v>
+      </c>
+      <c r="X191">
+        <v>2108.3000000000002</v>
+      </c>
+      <c r="Y191">
+        <v>2025.31</v>
+      </c>
+      <c r="Z191">
+        <v>1762.87</v>
       </c>
     </row>
   </sheetData>
@@ -15436,7 +16075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5179C7F0-00B1-42CF-AF11-C6D007A29719}">
   <dimension ref="B2:Z3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>

</xml_diff>